<commit_message>
updated gitignore for figures on bookdown website
</commit_message>
<xml_diff>
--- a/data/data_sheets/processed_summary_data/Site_Notes (version 1).xlsx
+++ b/data/data_sheets/processed_summary_data/Site_Notes (version 1).xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clang\Documents\USU\DF_Areas\data\data_sheets\processed_summary_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clang\Documents\USU\DF_Areas\debris_flow_stats\data\data_sheets\processed_summary_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D72F72C-0406-4847-A323-68E7B5343B49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D8B455C-1B6E-4657-8AD8-58926E1AFBDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" activeTab="1" xr2:uid="{58112664-7265-4281-A461-1CFD53DAA4AB}"/>
+    <workbookView xWindow="57390" yWindow="-210" windowWidth="29220" windowHeight="15900" xr2:uid="{58112664-7265-4281-A461-1CFD53DAA4AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="126">
   <si>
     <t>Site</t>
   </si>
@@ -150,9 +149,6 @@
     <t>Not clear in 2018, 2019 debris flow doesn't match with 2020 manual area</t>
   </si>
   <si>
-    <t>Y/N</t>
-  </si>
-  <si>
     <t>Possibly fluvial</t>
   </si>
   <si>
@@ -171,27 +167,18 @@
     <t>Very coarse looking in 2022</t>
   </si>
   <si>
-    <t>Toe recedes a ton by 2020, could be from the excavators. May not be a good site for toe erosion, although the initial df seems to have crossed river. Subcatch delineation is suspicious</t>
-  </si>
-  <si>
     <t>Shingle 2A</t>
   </si>
   <si>
     <t>Shingle 1A</t>
   </si>
   <si>
-    <t>Shingle 3A</t>
-  </si>
-  <si>
     <t>Lots of new sediment deposited in floodplain from 2013-2018. unlikely to be a new df, tried not to ID addition of sediment as original debris flow deposit in polygon. Area of bottleneck/aggradation?</t>
   </si>
   <si>
     <t>Big channel formation in 2019 in trib catch, lots of fan erosion. Toe erosion heavy as well</t>
   </si>
   <si>
-    <t>lots of sediment from fluvial transport. Hard to differentiate new sediment from eroded toe. Could be a good field site? Likely a bottleneck for sediment.</t>
-  </si>
-  <si>
     <t>heavily vegetated in 2013, extent of DF not clear. Risk of  overestimating, may not have made it to channel</t>
   </si>
   <si>
@@ -207,15 +194,6 @@
     <t>2021 imagery not clear at toe and most of the fan… large channel development on fan but can't delineate polygon. Omit 2021</t>
   </si>
   <si>
-    <t>Lake Fork 2A</t>
-  </si>
-  <si>
-    <t>""</t>
-  </si>
-  <si>
-    <t>use as channel initiation example? Fan erosion heavy</t>
-  </si>
-  <si>
     <t>2019 imagery clear, but toe obscured by vegetation. 2021 not clear</t>
   </si>
   <si>
@@ -237,33 +215,6 @@
     <t>West Valley 3</t>
   </si>
   <si>
-    <t>no channel to intersect</t>
-  </si>
-  <si>
-    <t>no channel intersection at toe</t>
-  </si>
-  <si>
-    <t>road at toe, unclear if it made it to channel</t>
-  </si>
-  <si>
-    <t>2019 imagery low resolution</t>
-  </si>
-  <si>
-    <t>2019 imagery unclear</t>
-  </si>
-  <si>
-    <t>no imagery available after 2013 in GEE</t>
-  </si>
-  <si>
-    <t>huge deposit but channel intersection is unclear, could be channel initiated</t>
-  </si>
-  <si>
-    <t>did not make it to channel. Highway at toe</t>
-  </si>
-  <si>
-    <t>unclear if it made it to channel</t>
-  </si>
-  <si>
     <t>Brian Head 5A</t>
   </si>
   <si>
@@ -381,18 +332,6 @@
     <t>i15_mm/.25h</t>
   </si>
   <si>
-    <t>not near channel</t>
-  </si>
-  <si>
-    <t>2021 too vegetated, omit 2021</t>
-  </si>
-  <si>
-    <t>no river, highway</t>
-  </si>
-  <si>
-    <t>no river</t>
-  </si>
-  <si>
     <t>too vegetated</t>
   </si>
   <si>
@@ -445,6 +384,39 @@
   </si>
   <si>
     <t>Trail Mountain, 2018</t>
+  </si>
+  <si>
+    <t>no delivery</t>
+  </si>
+  <si>
+    <t>Deposited on another fan (visible in 2015 -- pre-fire)</t>
+  </si>
+  <si>
+    <t>imagery unclear through 2021-2022</t>
+  </si>
+  <si>
+    <t>Clay Springs 3</t>
+  </si>
+  <si>
+    <t>Clay Springs 4</t>
+  </si>
+  <si>
+    <t>Clay Springs 5</t>
+  </si>
+  <si>
+    <t>highway</t>
+  </si>
+  <si>
+    <t>Trail Mountain 5A</t>
+  </si>
+  <si>
+    <t>2021 too vegetated, omit 2021, only 2 yrs of data</t>
+  </si>
+  <si>
+    <t>not enough images</t>
+  </si>
+  <si>
+    <t>no delivery, also road at toe</t>
   </si>
 </sst>
 </file>
@@ -814,7 +786,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -822,10 +794,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{030CF839-DFCE-462E-A1B1-10FDFFAB2A40}">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -860,15 +832,15 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.5">
@@ -876,13 +848,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -890,7 +862,10 @@
         <v>29</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.5">
@@ -898,10 +873,10 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.5">
@@ -909,320 +884,350 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>118</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="114.7" x14ac:dyDescent="0.5">
+        <v>119</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>120</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.5">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>29</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>37</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>29</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="43" x14ac:dyDescent="0.5">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="86" x14ac:dyDescent="0.5">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="C15" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="43" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:4" ht="86" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.5">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
-        <v>55</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E18" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="86" x14ac:dyDescent="0.5">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="57.35" x14ac:dyDescent="0.5">
+      <c r="A20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="86" x14ac:dyDescent="0.5">
+      <c r="A21" t="s">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B21" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C21" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A26" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A27" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A30" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A21" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A22" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
+    <row r="31" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A31" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="43" x14ac:dyDescent="0.5">
+      <c r="A32" t="s">
+        <v>22</v>
+      </c>
+      <c r="B32" t="s">
+        <v>29</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="114.7" x14ac:dyDescent="0.5">
+      <c r="A33" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A23" t="s">
-        <v>41</v>
-      </c>
-      <c r="B23" t="s">
+      <c r="C33" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="57.35" x14ac:dyDescent="0.5">
+      <c r="A34" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A24" t="s">
-        <v>23</v>
-      </c>
-      <c r="B24" t="s">
-        <v>29</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A25" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25" t="s">
-        <v>29</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A26" t="s">
-        <v>25</v>
-      </c>
-      <c r="B26" t="s">
-        <v>6</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A27" t="s">
-        <v>26</v>
-      </c>
-      <c r="B27" t="s">
-        <v>29</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A28" t="s">
-        <v>27</v>
-      </c>
-      <c r="B28" t="s">
-        <v>29</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A29" t="s">
-        <v>28</v>
-      </c>
-      <c r="B29" t="s">
-        <v>29</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="43" x14ac:dyDescent="0.5">
-      <c r="A30" t="s">
-        <v>22</v>
-      </c>
-      <c r="B30" t="s">
-        <v>29</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="114.7" x14ac:dyDescent="0.5">
-      <c r="A31" t="s">
+      <c r="C34" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="B31" t="s">
-        <v>6</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="57.35" x14ac:dyDescent="0.5">
-      <c r="A32" t="s">
-        <v>44</v>
-      </c>
-      <c r="B32" t="s">
-        <v>6</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="86" x14ac:dyDescent="0.5">
-      <c r="A33" t="s">
-        <v>46</v>
-      </c>
-      <c r="B33" t="s">
-        <v>29</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A34" t="s">
-        <v>62</v>
-      </c>
-      <c r="B34" t="s">
-        <v>29</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A35" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B35" t="s">
         <v>29</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A36" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B36" t="s">
         <v>29</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>117</v>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A37" t="s">
+        <v>57</v>
+      </c>
+      <c r="B37" t="s">
+        <v>29</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1231,7 +1236,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54894D0D-EE55-4B73-8C7C-8BDABF5DC1FB}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
@@ -1249,25 +1254,25 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="C1" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="F1" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="G1" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="H1" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.5">
@@ -1281,7 +1286,7 @@
         <v>43319</v>
       </c>
       <c r="D2" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="E2">
         <v>0.12</v>
@@ -1294,7 +1299,7 @@
         <v>2.2897823659124059E-2</v>
       </c>
       <c r="H2" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.5">
@@ -1308,7 +1313,7 @@
         <v>43318</v>
       </c>
       <c r="D3" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="E3">
         <v>0.12</v>
@@ -1321,7 +1326,7 @@
         <v>0.13397967064008295</v>
       </c>
       <c r="H3" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.5">
@@ -1335,7 +1340,7 @@
         <v>43319</v>
       </c>
       <c r="D4" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="E4">
         <v>0.12</v>
@@ -1348,12 +1353,12 @@
         <v>2.1561429861640638E-4</v>
       </c>
       <c r="H4" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="B5" s="2">
         <v>42925</v>
@@ -1362,7 +1367,7 @@
         <v>43319</v>
       </c>
       <c r="D5" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="E5">
         <v>0.12</v>
@@ -1375,12 +1380,12 @@
         <v>8.1324583548123539E-2</v>
       </c>
       <c r="H5" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B6" s="2">
         <v>43303</v>
@@ -1389,7 +1394,7 @@
         <v>43362</v>
       </c>
       <c r="D6" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="E6">
         <v>0.16</v>
@@ -1405,12 +1410,12 @@
         <v>2</v>
       </c>
       <c r="I6" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="B7" s="2">
         <v>43303</v>
@@ -1419,7 +1424,7 @@
         <v>43362</v>
       </c>
       <c r="D7" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="E7">
         <v>0.16</v>
@@ -1432,7 +1437,7 @@
         <v>1.4347517556886237E-2</v>
       </c>
       <c r="H7" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.5">
@@ -1446,7 +1451,7 @@
         <v>43362</v>
       </c>
       <c r="D8" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="E8">
         <v>0.16</v>
@@ -1473,7 +1478,7 @@
         <v>43362</v>
       </c>
       <c r="D9" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="E9">
         <v>0.16</v>
@@ -1500,7 +1505,7 @@
         <v>43362</v>
       </c>
       <c r="D10" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="E10">
         <v>0.16</v>
@@ -1527,7 +1532,7 @@
         <v>43370</v>
       </c>
       <c r="D11" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="E11">
         <v>0.01</v>
@@ -1540,12 +1545,12 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="H11" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B12" s="2">
         <v>43361</v>
@@ -1554,7 +1559,7 @@
         <v>43370</v>
       </c>
       <c r="D12" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="E12">
         <v>0.01</v>
@@ -1567,7 +1572,7 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="H12" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.5">
@@ -1581,7 +1586,7 @@
         <v>43370</v>
       </c>
       <c r="D13" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="E13">
         <v>0.01</v>
@@ -1594,7 +1599,7 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="H13" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.5">
@@ -1608,7 +1613,7 @@
         <v>41425</v>
       </c>
       <c r="D14" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="E14">
         <v>0.11</v>
@@ -1621,12 +1626,12 @@
         <v>2.170630968936104E-2</v>
       </c>
       <c r="H14" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B15" s="2">
         <v>41097</v>
@@ -1635,7 +1640,7 @@
         <v>41425</v>
       </c>
       <c r="D15" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="E15">
         <v>0.11</v>
@@ -1648,12 +1653,12 @@
         <v>4.3249016770476592E-3</v>
       </c>
       <c r="H15" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="B16" s="2">
         <v>41097</v>
@@ -1662,7 +1667,7 @@
         <v>41425</v>
       </c>
       <c r="D16" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="E16">
         <v>0.11</v>
@@ -1675,12 +1680,12 @@
         <v>8.4406140384535259E-3</v>
       </c>
       <c r="H16" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B17" s="2">
         <v>41102</v>
@@ -1689,7 +1694,7 @@
         <v>41430</v>
       </c>
       <c r="D17" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="E17">
         <v>0.22</v>
@@ -1702,12 +1707,12 @@
         <v>0.15</v>
       </c>
       <c r="H17" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B18" s="2">
         <v>41470</v>
@@ -1716,7 +1721,7 @@
         <v>42209</v>
       </c>
       <c r="D18" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="E18">
         <v>0.31</v>
@@ -1729,12 +1734,12 @@
         <v>0.17</v>
       </c>
       <c r="H18" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="B19" s="2">
         <v>43268</v>
@@ -1743,7 +1748,7 @@
         <v>43355</v>
       </c>
       <c r="D19" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="E19">
         <v>0.01</v>
@@ -1756,12 +1761,12 @@
         <v>1.4397745921012549E-2</v>
       </c>
       <c r="H19" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="B20" s="2">
         <v>43268</v>
@@ -1770,7 +1775,7 @@
         <v>43355</v>
       </c>
       <c r="D20" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="E20">
         <v>0.01</v>
@@ -1783,12 +1788,12 @@
         <v>1.5458354998179248E-2</v>
       </c>
       <c r="H20" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="B21" s="2">
         <v>43268</v>
@@ -1797,7 +1802,7 @@
         <v>43355</v>
       </c>
       <c r="D21" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="E21">
         <v>0.01</v>
@@ -1810,12 +1815,12 @@
         <v>2.32608085232675E-2</v>
       </c>
       <c r="H21" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="B22" s="2">
         <v>43268</v>
@@ -1824,7 +1829,7 @@
         <v>43355</v>
       </c>
       <c r="D22" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="E22">
         <v>0.01</v>
@@ -1834,18 +1839,18 @@
         <v>0.254</v>
       </c>
       <c r="H22" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="C23" s="2">
         <v>40809</v>
       </c>
       <c r="D23" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="E23">
         <v>0.4</v>
@@ -1860,7 +1865,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A24" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="C24" s="2">
         <v>40809</v>
@@ -1872,7 +1877,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A25" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="C25" s="2">
         <v>40809</v>
@@ -1884,7 +1889,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A26" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="C26" s="2">
         <v>40809</v>
@@ -1896,7 +1901,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A27" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="C27" s="2">
         <v>40809</v>
@@ -1908,7 +1913,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A28" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="C28" s="2">
         <v>40809</v>
@@ -1920,7 +1925,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A29" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="C29" s="2">
         <v>40809</v>
@@ -1932,7 +1937,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A30" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="C30" s="2">
         <v>40809</v>
@@ -1957,10 +1962,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF28A333-BCD1-4FF9-BD35-55E009A51953}">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection sqref="A1:D34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1974,13 +1979,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.5">
@@ -1988,7 +1993,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
       <c r="C2">
         <v>37.741477000000003</v>
@@ -1999,10 +2004,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="B3" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
       <c r="C3">
         <v>37.767022900000001</v>
@@ -2013,10 +2018,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
-        <v>128</v>
+        <v>108</v>
       </c>
       <c r="C4">
         <v>40.096805000000003</v>
@@ -2027,10 +2032,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="B5" t="s">
-        <v>128</v>
+        <v>108</v>
       </c>
       <c r="C5">
         <v>40.106735899999997</v>
@@ -2044,7 +2049,7 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>128</v>
+        <v>108</v>
       </c>
       <c r="C6">
         <v>40.120918000000003</v>
@@ -2058,7 +2063,7 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>128</v>
+        <v>108</v>
       </c>
       <c r="C7">
         <v>40.120640000000002</v>
@@ -2072,7 +2077,7 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>128</v>
+        <v>108</v>
       </c>
       <c r="C8">
         <v>40.121447000000003</v>
@@ -2086,7 +2091,7 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
       <c r="C9">
         <v>39.962445000000002</v>
@@ -2097,10 +2102,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B10" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
       <c r="C10">
         <v>39.946106</v>
@@ -2114,7 +2119,7 @@
         <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
       <c r="C11">
         <v>39.941927</v>
@@ -2128,7 +2133,7 @@
         <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="C12">
         <v>39.541237000000002</v>
@@ -2139,10 +2144,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B13" t="s">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="C13">
         <v>39.552032500000003</v>
@@ -2153,10 +2158,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="B14" t="s">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="C14">
         <v>39.561988100000001</v>
@@ -2167,10 +2172,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>131</v>
+        <v>111</v>
       </c>
       <c r="C15">
         <v>37.4360906</v>
@@ -2181,10 +2186,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B16" t="s">
-        <v>131</v>
+        <v>111</v>
       </c>
       <c r="C16">
         <v>37.450863200000001</v>
@@ -2195,10 +2200,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="B17" t="s">
-        <v>134</v>
+        <v>114</v>
       </c>
       <c r="C17">
         <v>39.424022999999998</v>
@@ -2209,776 +2214,248 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="B18" t="s">
-        <v>134</v>
-      </c>
-      <c r="C18">
-        <v>39.423610799999999</v>
-      </c>
-      <c r="D18" s="4">
-        <v>-111.1504207</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="D18" s="4"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="B19" t="s">
-        <v>134</v>
-      </c>
-      <c r="C19">
-        <v>39.425620100000003</v>
-      </c>
-      <c r="D19" s="4">
-        <v>-111.1600538</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="D19" s="4"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="B20" t="s">
-        <v>132</v>
-      </c>
-      <c r="C20">
-        <v>38.501213999999997</v>
-      </c>
-      <c r="D20">
-        <v>-112.453485</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="D20" s="4"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
-        <v>83</v>
+        <v>122</v>
       </c>
       <c r="B21" t="s">
-        <v>132</v>
-      </c>
-      <c r="C21">
-        <v>38.504078</v>
-      </c>
-      <c r="D21">
-        <v>-112.456199</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="D21" s="4"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="B22" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="C22">
-        <v>38.504983000000003</v>
+        <v>38.501213999999997</v>
       </c>
       <c r="D22">
-        <v>-112.456048</v>
+        <v>-112.453485</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
-        <v>118</v>
+        <v>67</v>
       </c>
       <c r="B23" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="C23">
-        <v>38.514330000000001</v>
+        <v>38.504078</v>
       </c>
       <c r="D23">
-        <v>-112.459064</v>
+        <v>-112.456199</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A24" t="s">
-        <v>119</v>
+        <v>68</v>
       </c>
       <c r="B24" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="C24">
-        <v>38.519455999999998</v>
+        <v>38.504983000000003</v>
       </c>
       <c r="D24">
-        <v>-112.456953</v>
+        <v>-112.456048</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A25" t="s">
-        <v>120</v>
+        <v>98</v>
       </c>
       <c r="B25" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="C25">
-        <v>38.540412000000003</v>
+        <v>38.514330000000001</v>
       </c>
       <c r="D25">
-        <v>-112.448812</v>
+        <v>-112.459064</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A26" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="B26" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="C26">
-        <v>38.514330000000001</v>
+        <v>38.519455999999998</v>
       </c>
       <c r="D26">
-        <v>-112.459064</v>
+        <v>-112.456953</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A27" t="s">
-        <v>122</v>
+        <v>100</v>
       </c>
       <c r="B27" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="C27">
-        <v>38.519455999999998</v>
+        <v>38.540412000000003</v>
       </c>
       <c r="D27">
-        <v>-112.456953</v>
+        <v>-112.448812</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A28" t="s">
-        <v>123</v>
+        <v>101</v>
       </c>
       <c r="B28" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="C28">
-        <v>38.519455999999998</v>
+        <v>38.514330000000001</v>
       </c>
       <c r="D28">
-        <v>-112.456953</v>
+        <v>-112.459064</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A29" t="s">
-        <v>124</v>
+        <v>102</v>
       </c>
       <c r="B29" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="C29">
-        <v>38.540412000000003</v>
+        <v>38.519455999999998</v>
       </c>
       <c r="D29">
-        <v>-112.448812</v>
+        <v>-112.456953</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A30" t="s">
-        <v>88</v>
+        <v>103</v>
       </c>
       <c r="B30" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="C30">
-        <v>38.497454400000002</v>
-      </c>
-      <c r="D30" s="4">
-        <v>-111.1504207</v>
+        <v>38.519455999999998</v>
+      </c>
+      <c r="D30">
+        <v>-112.456953</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A31" t="s">
-        <v>125</v>
+        <v>104</v>
       </c>
       <c r="B31" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="C31">
-        <v>38.521416000000002</v>
+        <v>38.540412000000003</v>
       </c>
       <c r="D31">
-        <v>-112.48801</v>
+        <v>-112.448812</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A32" t="s">
-        <v>126</v>
+        <v>72</v>
       </c>
       <c r="B32" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="C32">
-        <v>38.521416000000002</v>
-      </c>
-      <c r="D32">
-        <v>-112.48801</v>
+        <v>38.497454400000002</v>
+      </c>
+      <c r="D32" s="4">
+        <v>-111.1504207</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A33" t="s">
-        <v>9</v>
+        <v>105</v>
       </c>
       <c r="B33" t="s">
-        <v>133</v>
-      </c>
-      <c r="C33" s="6">
-        <v>39.950797999999999</v>
+        <v>112</v>
+      </c>
+      <c r="C33">
+        <v>38.521416000000002</v>
       </c>
       <c r="D33">
-        <v>-111.34931899999999</v>
+        <v>-112.48801</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A34" t="s">
+        <v>106</v>
+      </c>
+      <c r="B34" t="s">
+        <v>112</v>
+      </c>
+      <c r="C34">
+        <v>38.521416000000002</v>
+      </c>
+      <c r="D34">
+        <v>-112.48801</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A35" t="s">
+        <v>9</v>
+      </c>
+      <c r="B35" t="s">
+        <v>113</v>
+      </c>
+      <c r="C35" s="6">
+        <v>39.950797999999999</v>
+      </c>
+      <c r="D35">
+        <v>-111.34931899999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A36" t="s">
         <v>10</v>
       </c>
-      <c r="B34" t="s">
-        <v>133</v>
-      </c>
-      <c r="C34">
+      <c r="B36" t="s">
+        <v>113</v>
+      </c>
+      <c r="C36">
         <v>39.953975</v>
       </c>
-      <c r="D34">
+      <c r="D36">
         <v>-111.347712</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61CE8127-8955-4C87-A2AE-7C7B3D3217F5}">
-  <dimension ref="A1:F30"/>
-  <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24:C24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
-  <cols>
-    <col min="1" max="1" width="25.234375" customWidth="1"/>
-    <col min="3" max="3" width="20.05859375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="143.35" x14ac:dyDescent="0.5">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>37.747757999999997</v>
-      </c>
-      <c r="C2">
-        <v>-112.788707</v>
-      </c>
-      <c r="D2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>37.741477000000003</v>
-      </c>
-      <c r="C3">
-        <v>-112.79320800000001</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>37.724361999999999</v>
-      </c>
-      <c r="C4">
-        <v>-112.706177</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>37.758555999999999</v>
-      </c>
-      <c r="C5">
-        <v>-112.79405199999999</v>
-      </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" ht="57.35" x14ac:dyDescent="0.5">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6">
-        <v>39.356532999999999</v>
-      </c>
-      <c r="C6">
-        <v>-112.164818</v>
-      </c>
-      <c r="D6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" ht="57.35" x14ac:dyDescent="0.5">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7">
-        <v>39.33334</v>
-      </c>
-      <c r="C7">
-        <v>-112.150673</v>
-      </c>
-      <c r="D7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8">
-        <v>39.950797999999999</v>
-      </c>
-      <c r="C8">
-        <v>-111.34931899999999</v>
-      </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9">
-        <v>39.953975</v>
-      </c>
-      <c r="C9">
-        <v>-111.347712</v>
-      </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10">
-        <v>40.120918000000003</v>
-      </c>
-      <c r="C10">
-        <v>-110.744614</v>
-      </c>
-      <c r="D10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11">
-        <v>40.114964000000001</v>
-      </c>
-      <c r="C11">
-        <v>-110.812256</v>
-      </c>
-      <c r="D11" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="71.7" x14ac:dyDescent="0.5">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12">
-        <v>40.118462000000001</v>
-      </c>
-      <c r="C12">
-        <v>-110.829193</v>
-      </c>
-      <c r="D12" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="129" x14ac:dyDescent="0.5">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13">
-        <v>40.120640000000002</v>
-      </c>
-      <c r="C13">
-        <v>-110.79077100000001</v>
-      </c>
-      <c r="D13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="272.35000000000002" x14ac:dyDescent="0.5">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14">
-        <v>40.121447000000003</v>
-      </c>
-      <c r="C14">
-        <v>-110.834881</v>
-      </c>
-      <c r="D14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15">
-        <v>39.962445000000002</v>
-      </c>
-      <c r="C15">
-        <v>-111.458642</v>
-      </c>
-      <c r="D15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" ht="71.7" x14ac:dyDescent="0.5">
-      <c r="A16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16">
-        <v>39.966935999999997</v>
-      </c>
-      <c r="C16">
-        <v>-111.45669700000001</v>
-      </c>
-      <c r="D16" t="s">
-        <v>29</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:6" ht="243.7" x14ac:dyDescent="0.5">
-      <c r="A17" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17">
-        <v>39.941927</v>
-      </c>
-      <c r="C17">
-        <v>-111.52309200000001</v>
-      </c>
-      <c r="D17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="1:6" ht="143.35" x14ac:dyDescent="0.5">
-      <c r="A18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18">
-        <v>39.892184999999998</v>
-      </c>
-      <c r="C18">
-        <v>-111.536011</v>
-      </c>
-      <c r="D18" t="s">
-        <v>29</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="1:6" ht="71.7" x14ac:dyDescent="0.5">
-      <c r="A19" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19">
-        <v>39.953434000000001</v>
-      </c>
-      <c r="C19">
-        <v>-111.529686</v>
-      </c>
-      <c r="D19" t="s">
-        <v>29</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20">
-        <v>39.541237000000002</v>
-      </c>
-      <c r="C20">
-        <v>-111.16181899999999</v>
-      </c>
-      <c r="D20" t="s">
-        <v>6</v>
-      </c>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="1:6" ht="186.35" x14ac:dyDescent="0.5">
-      <c r="A21" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21">
-        <v>37.430881749999998</v>
-      </c>
-      <c r="C21">
-        <v>-112.60078590000001</v>
-      </c>
-      <c r="D21" t="s">
-        <v>29</v>
-      </c>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="86" x14ac:dyDescent="0.5">
-      <c r="A22" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22">
-        <v>39.982624000000001</v>
-      </c>
-      <c r="C22">
-        <v>-111.212959</v>
-      </c>
-      <c r="D22" t="s">
-        <v>29</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="1:6" ht="57.35" x14ac:dyDescent="0.5">
-      <c r="A23" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23">
-        <v>39.998111999999999</v>
-      </c>
-      <c r="C23">
-        <v>-111.215523</v>
-      </c>
-      <c r="D23" t="s">
-        <v>29</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="1:6" ht="86" x14ac:dyDescent="0.5">
-      <c r="A24" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24">
-        <v>39.424022999999998</v>
-      </c>
-      <c r="C24">
-        <v>-111.156711</v>
-      </c>
-      <c r="D24" t="s">
-        <v>6</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="100.35" x14ac:dyDescent="0.5">
-      <c r="A25" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25">
-        <v>39.423344</v>
-      </c>
-      <c r="C25">
-        <v>-111.14059399999999</v>
-      </c>
-      <c r="D25" t="s">
-        <v>29</v>
-      </c>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="129" x14ac:dyDescent="0.5">
-      <c r="A26" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26">
-        <v>39.404434000000002</v>
-      </c>
-      <c r="C26">
-        <v>-111.13722199999999</v>
-      </c>
-      <c r="D26" t="s">
-        <v>29</v>
-      </c>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="100.35" x14ac:dyDescent="0.5">
-      <c r="A27" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27">
-        <v>39.461922000000001</v>
-      </c>
-      <c r="C27">
-        <v>-111.18002300000001</v>
-      </c>
-      <c r="D27" t="s">
-        <v>29</v>
-      </c>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="57.35" x14ac:dyDescent="0.5">
-      <c r="A28" t="s">
-        <v>62</v>
-      </c>
-      <c r="B28">
-        <v>37.450812999999997</v>
-      </c>
-      <c r="C28">
-        <v>-113.437439</v>
-      </c>
-      <c r="D28" t="s">
-        <v>29</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="43" x14ac:dyDescent="0.5">
-      <c r="A29" t="s">
-        <v>63</v>
-      </c>
-      <c r="B29">
-        <v>37.448124</v>
-      </c>
-      <c r="C29">
-        <v>-113.406265</v>
-      </c>
-      <c r="D29" t="s">
-        <v>29</v>
-      </c>
-      <c r="E29" t="s">
-        <v>38</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="86" x14ac:dyDescent="0.5">
-      <c r="A30" t="s">
-        <v>64</v>
-      </c>
-      <c r="B30">
-        <v>37.449370999999999</v>
-      </c>
-      <c r="C30">
-        <v>-113.415977</v>
-      </c>
-      <c r="D30" t="s">
-        <v>29</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -2987,7 +2464,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA0062C2-A70C-4E37-A1F3-AFFA25865900}">
   <dimension ref="A1:B30"/>
   <sheetViews>
@@ -3006,7 +2483,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.5">
@@ -3014,7 +2491,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.5">
@@ -3035,7 +2512,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="B5" t="s">
         <v>29</v>
@@ -3043,15 +2520,15 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B6" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="B7" t="s">
         <v>29</v>
@@ -3086,12 +2563,12 @@
         <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B12" t="s">
         <v>29</v>
@@ -3115,15 +2592,15 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B15" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="B16" t="s">
         <v>29</v>
@@ -3131,23 +2608,23 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B17" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B18" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="B19" t="s">
         <v>29</v>
@@ -3155,7 +2632,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="B20" t="s">
         <v>29</v>
@@ -3163,7 +2640,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="B21" t="s">
         <v>29</v>
@@ -3171,7 +2648,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="B22" t="s">
         <v>29</v>
@@ -3179,7 +2656,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="B23" t="s">
         <v>29</v>
@@ -3187,15 +2664,15 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A24" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="B24" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A25" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="B25" t="s">
         <v>29</v>
@@ -3203,23 +2680,23 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A26" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="B26" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A27" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="B27" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A28" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="B28" t="s">
         <v>29</v>
@@ -3227,7 +2704,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A29" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="B29" t="s">
         <v>29</v>
@@ -3235,10 +2712,10 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A30" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="B30" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>